<commit_message>
Get daily reddit data: Tue Apr 29 08:13:31 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_04.xlsx
+++ b/data/collected_data/2025_05_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C494"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3287 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1kaiaof</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaiaof</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1kaiaju</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Matching my nails to my coloring pages 🥰❤️ I never had blue nails before, but these feel so right!</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fr0kv8rd9qxe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1kagx8h</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>First mani in a while..</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0u5o427spxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1kagjyi</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Chrome powder?</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kagjyi/chrome_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1kagjt4</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Before/after.</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kagjt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1kagf8w</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Got GelX done for the first time and it’s a game changer for sure!</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/186ezmu5mpxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1kagb38</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Still learning and stoked</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kagb38</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1kag9wn</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Care for natural nails</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kag9wn</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1kag0hl</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Looks weird but not sure what's wrong</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kag0hl</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1kafyx2</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kafyx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1kafvil</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Ready for transformation</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s37n21zufpxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1kafo76</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Redid my nails after salon did poor job</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kafo76</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1kafns1</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>about a month, maybe two, i had press on nails.. and they damaged my nails from not putting them on correctly. (sorry for some of the horrible blurry photos my camera SUCKS) but i tried to get every angle</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kafns1</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1kaev9g</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>is this worth $80?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaev9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1kac95l</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Press on nail removal</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5vjrvrzfoxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1kadncj</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>What do I ask for to get what I want?</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnv5bs12toxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1kaep5k</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>How do you find a decent nail salon that takes cleanliness seriously ?</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kaep5k/how_do_you_find_a_decent_nail_salon_that_takes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1kaervf</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Cured gel overflow pls help</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kaervf/cured_gel_overflow_pls_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1kaei5v</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Are these cute?!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6q8kjjf1pxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1kae46w</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>My first time getting my nails done!</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/54pz5cckxoxe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1kadlx5</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>not sure if this is the right place to post this..</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kadlx5/not_sure_if_this_is_the_right_place_to_post_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1kacocp</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Glamnetic Nails: Tips</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwyx0b6xjoxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1kacnss</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Starting my nails journey</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kacnss/starting_my_nails_journey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1kacf3w</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Rate my beginner nail sets</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kacf3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1kabutx</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>the nails I did today, I'm improving</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/skdyqv8dcoxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1kabm0b</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Got my ideal "my nails but better"!</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/si8uh7s3aoxe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1kabj7q</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Pink nails by me</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kabj7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1kabi93</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Do they look like teeth??</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xl70evq59oxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1kab8ow</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Funny bunny w Chrome</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kab8ow</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1kaaz4m</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>The beginning - Now.☺️</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2m5h2fff4oxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1kaazap</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>I went for bold colors.. was it too bold?</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40ln6xqg4oxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1kaawm1</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>new fresh set!!</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaawm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1kaaknd</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>What do you think? I’m a total mani newb.</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaaknd</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1kaak35</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Last year's birthday nails! Acrylic with gel polish.</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zj5g9dcr0oxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1kaajlr</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Are press on nails actually worth it instead of salon gels?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kaajlr/are_press_on_nails_actually_worth_it_instead_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1kaaaq1</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Fave press ons</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3b0c3e5iynxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1ka9tii</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>i absolutely hate my new nails</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j0tscmedunxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1ka9tnf</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Strawberries 🍓</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6c3h4keunxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1ka8m6o</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Is this fungus??</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/01kgagpeknxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1ka8gud</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Any way I can prevent this type of cuticle?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka8gud</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1ka88pf</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>When your nails hit harder than your jewelry</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49vr81rfhnxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1ka7gy6</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Decisions, decisions…</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka7gy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1ka5xas</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Stopped trimming nail corners. How so I fix this?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unk64g3szmxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1ka6ugs</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>The superglue method just changed everything for my nails!!</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka6ugs</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1ka6vcb</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Butter yellow for the spring 💛🌻</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apw9xbbt6nxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1ka6upk</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Who else loves a matching set? 🍒</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nca5q47q6nxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1ka6unr</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Sparkly spring 🌸🦋</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vt7as38p6nxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1ka6ro4</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqrw50k36nxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1ka6kiy</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Builder gel help!</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o962g4rl4nxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1ka5z4e</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Which shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka5z4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1ka5vn5</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Do these look too long for me? Press ons</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka5vn5</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1ka5qrz</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Can I get acrylics with my broken nail?</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vpqjw7reymxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1ka5mu0</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Labubu Nails these took me 60 hours to complete but so worth it 🥰</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka5mu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1ka58bh</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>I love my Nail Lady</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awk2bmtkumxe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1ka5dwu</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Thinking about doing nails/ press ons</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka5dwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1ka507d</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>To cut or not to cut, that is the question</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka507d</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1ka4xrp</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>What gel nail kit do you recommend?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ka4xrp/what_gel_nail_kit_do_you_recommend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1ka4snw</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Finally a pastel yellow!</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gsd3digrmxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1ka4em2</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Newest set and I’m a little obsessed</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s73unv6komxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1ka4ar0</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Central Texas wildflower nails 🌼💐</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka4ar0</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1ka48dz</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Are these too far from the cuticle?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka48dz</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1ka3xrk</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Shape Help</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka3xrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1ka328v</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Dnd pastel purple …</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h608eiloemxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1ka2luu</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Crusty nails 😭</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka2luu</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1ka2dl6</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Best milky, sheer light pink gel</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ka2dl6/best_milky_sheer_light_pink_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1ka3u0g</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Trying something different, I don't usually use this style</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rbaysyq7kmxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1ka3mb7</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Just got my nails done yesterday!</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka3mb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1ka3akc</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Do these look as bad as I think they do?</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka3akc</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1ka33im</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>gel manicure : self done</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka33im</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1ka2wjm</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>🧡 ILNP Atomic Sherbet</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka2wjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1ka2rw5</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Reminds me of posts I would see on this subreddit 😆</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oblq8a6jcmxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1ka2f48</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Might be my new favorite set 💖</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mkjrv70amxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1ka1cup</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>How to avoid these harsh lines in my nails after gel polish</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka1cup</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1ka1lym</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Barbie California dream</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka1lym</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1ka1wgg</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Thoughts and Ideas for my next theme?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka1wgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1ka2446</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Glass cat eye nails for $20</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0pu6mg8t7mxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1ka1vy7</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>I absolutely love my nails! First time doing chrome!</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka1vy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1ka1ojt</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Green design! 💚✨</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka1ojt</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1ka1ld2</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>bright and colorful spring set</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka1ld2</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1ka1gdx</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Gel-X extensions popped off after 1 week and left my nails flaky/peeling. Should I cut them down?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka1gdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1ka1ae6</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>To all my seasoned nail ladies, please share your tips for the newbies.</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ka1ae6/to_all_my_seasoned_nail_ladies_please_share_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1ka0ydl</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Death Valley Nails</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ka0ydl/death_valley_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1ka0rts</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>My nail place is 🔥</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka0rts</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1ka0qnq</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Sparkly flowers 💐</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4dlhxj2ylxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1ka0fpf</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Nail girlies pls help!!</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka0fpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1ka0jhj</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>How to write with long nails!</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7x6keb6pwlxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1k9pah4</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Clear nails</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k9pah4/clear_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1k9rmjq</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Looking for peach gold nail polish</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvvhbg5nrjxe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1k9rn2w</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>How to use press on nails on nails like this?</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5h0s8wrtrjxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1k9sboa</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>First time doing tips and gel</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6y3gh6zyzjxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1k9vmx3</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Trying nail glue for press ons instead of glue tabs for the first time, what am I doing wrong??</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3yul4qdxvkxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1ka07p2</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>I don’t like red.. but this one got me 🥵</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qi0w6z27ulxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1k9y547</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Please help need inspo for prom nails Im not good at this kind of stuff!</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9y547</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1k9z2w6</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>French i did v my friend chronicnailz on ig</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9z2w6</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1ka04rv</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>jelly rainbow set i did last night 🌈</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka04rv</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1ka0179</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>I think this is Royal Purple 👑 💜✨</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gcw32kduslxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1ka006n</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Best pearl chrome powder?</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ka006n/best_pearl_chrome_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1k9zvwr</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>She delivered 💥</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9zvwr</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1k9zs9i</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>loving my birthday nails 🥰🥰</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6y6evhwqlxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1k9zjhb</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Gel X removal cost</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k9zjhb/gel_x_removal_cost/</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1kaiewy</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>You're Making us Look Bad</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaiewy</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1kafqh9</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Finally wearing color again</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2fbzdu8aepxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1kadq8k</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Am I the only one that actually likes the current OPI Nail Envy formula?</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kadq8k/am_i_the_only_one_that_actually_likes_the_current/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1kadnwr</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>How do you make designs on your nails? With fabric paint or enamel?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kadnwr/how_do_you_make_designs_on_your_nails_with_fabric/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1kadn4a</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>WHY!? Nails Inc Glowing my way formula changed!</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kadn4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1kacpqo</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Crystal Knockout Fly Owl is a thick, thick polish.</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4e4yk8z9koxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1kabtfw</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>My favorite color is whatever this is</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xm96v9m0coxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1kaboap</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Thoughts</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaboap</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1kabepj</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Thermal - Flakies - Clear Base</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kabepj/thermal_flakies_clear_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1kabamk</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Fields of Lavender is stunning</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/otdzwl0a7oxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1kab2ki</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Can someone explain Ethereal prototypes to me?</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kab2ki/can_someone_explain_ethereal_prototypes_to_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1kaav8j</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Shell We Dance? 🐚</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaav8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1kaao3k</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Matching with my drink 🌸</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dk6j6z4q1oxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1ka94vn</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>First flakies, I am a believer</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka94vn</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1ka8x3h</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Swatch Request: Manucurist Active Glow</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ka8x3h/swatch_request_manucurist_active_glow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1ka8u35</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>New Bottle, New Brush</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ha7w93g7mnxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1ka82gx</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>This morning was my first time ever seeing Lurid’s Bajo Las Frondas in sunlight ✨🌴☀️</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka82gx</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1ka7tfu</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Please help me understand magnetic fields</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnymkik3enxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1ka7evx</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Black/gray jelly recs?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ka7evx/blackgray_jelly_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1ka6ug0</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>📬 Double Nail Mail Day! 💅</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka6ug0</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1ka6u34</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Practicing my freehand skills</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka6u34</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1ka6qlc</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>I bought a Clionadh mystery box - here's what I got!</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka6qlc</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1ka6cb0</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Nailtiques Formula 2 Plus</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ka6cb0/nailtiques_formula_2_plus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1ka5xoj</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Didn’t mean to match but I love it</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka5xoj</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1ka5i1f</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Will there be an additional tariff to the US</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ka5i1f/will_there_be_an_additional_tariff_to_the_us/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1ka4tao</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Spirit🫧🤍</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v8nxo7tjrmxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1ka4fh4</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Mooncat “pandemonium”</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka4fh4</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1ka4a9u</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Y’all already know what it is🍄🍄🍄🍄</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ch879ednnmxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1ka46r5</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>First time wearing this since purchasing during Black Friday! She’s gorgeous!</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hrifxhymmxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1ka35a5</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Zoinkies Batman! What a gorgeous color!</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dk6sa6pafmxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1ka304k</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>ahhhhhhh.</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka304k</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1ka2xlb</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Swatch dots bottle question</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka2xlb</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1ka2vus</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>🧡 ILNP Atomic Sherbet</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka2vus</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1ka2pja</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Nail work ahead</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4iamxekbmxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1ka2ixc</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>springy simple one</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka2ixc</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1ka2d74</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>neutral, but make it glittery ✨</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka2d74</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1ka1i28</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Question re: acetone additives</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ka1i28/question_re_acetone_additives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1ka1hvq</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>... lurid might be the goat</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka1hvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1ka0huw</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Lyn B Designs -Enchanted Aura</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pwr22xwbwlxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1ka0ebq</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>It’s giving ✨pickle juice✨</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0slg85mvlxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1ka09fv</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Let’s go Red and Blue ❤️💙</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka09fv</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1k9zztd</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>April manis! 🌦️</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9zztd</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1k9zx6u</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>What am I missing?</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojqqbw80slxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1k9zlfo</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>radish colored gel polish?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k9zlfo/radish_colored_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1k9z2b0</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Finally got the hang of my horseshoe magnet</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zjsp1i0vllxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1k9yy7k</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>cirque eb &amp; flow 🩵💜</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9yy7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1k9ym2f</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>My little PPU haul</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xge3c1nilxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1k9yg3n</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Your favorite white crème?</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k9yg3n/your_favorite_white_crème/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1k9xwfi</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>💚 bog dweller 💚</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4vys3tz5dlxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1k9xudc</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Yellow lovers rejoice! This beauty is “What’s That In The Mustard?” by Broken Pixel Polish 💛</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9xudc</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1k9xfno</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Bought cheap stuff to start but what should I slowly stockpile?</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9xfno</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1k9x7q7</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>april/march manis, starting with current. which shape do we like best?</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9x7q7</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1k9wzgv</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Does anyone know of a topper similar to Cracked Taco by Holo Taco? Just wondering if I have to go ahead and buy it since it’s being retired…. I would love to have the option of adding that black cracked look</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k9wzgv/does_anyone_know_of_a_topper_similar_to_cracked/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1k9wuvt</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Kb Shimmer Aim to Breeze! New favorite ever. You will have to pry this one from my cold dead hands 💀🤘🏻</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9wuvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1k9wtho</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Broken nail update</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9wtho</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1k9wskg</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Sassy Sauce 🤩</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/abko4n315lxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1k9whhq</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Same Lie Lilac</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3eqlh1o2lxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1k9wdm8</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Pretty Fly for a Cacti</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4oovz59u1lxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1k9w8zn</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>What do you do?</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dwc3d0w0lxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1k9vcm6</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>new fave spring red</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9vcm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1k9t89u</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Dry and gross cuticles… where to begin?</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k9t89u/dry_and_gross_cuticles_where_to_begin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1k9sunh</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>My Last Mooncat Haul</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9sunh</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1k9ssqa</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Another one of my many purple nail polishes.</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9ssqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1k9shua</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Cirque Colors Jellies</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9shua</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1k9ryw4</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Looking for a replacement for Manglaze matte top coat</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9ryw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1k9rugp</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k9rugp/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1k9rlfc</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>My nails scream 🌈 rainbow🌈</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9uzcun8rjxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1k9r0vt</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Emily de Molly‘s Lament in various lightings 🥰</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9r0vt</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1kaihpv</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Is there anything that can be improved about the way this specific phrase looks?</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaihpv</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1kadp8y</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>nails i did this week in class!</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1q08ubktoxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1kadexj</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Beachy mermaid nails! 🧜‍♀️✨🐚</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hj24cjduqoxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1kabpxk</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>what does protein bonder ACTUALLY do??</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kabpxk/what_does_protein_bonder_actually_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1kabm36</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Fresh set, coming in sassy.</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7znjd1q4aoxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1kaay2h</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>First set on my actual nails</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaay2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1kaa794</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Second time doing nails like this. 1/10?</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaa794</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1ka97wb</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>First Time Using 3D Charms! Pink Bow Nails!</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltarbjwdpnxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1ka8t8r</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>chromakopia nails, what do you think?</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hl5b71ivlnxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1ka6fil</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Matte top coat for Aura pigments?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ka6fil/matte_top_coat_for_aura_pigments/</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1ka2jns</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>My new nails with 3D strawberries</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka2jns</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1k9f8x0</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>How’d I do?</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9f8x0</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1k9fao9</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Is it nice? Can you give me Star 5 out of ???</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7iz54646gxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1k9pode</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Finally finished these nails today!</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9pode</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1ka1jvi</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Barbie California dream</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ka1jvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1k9y1i9</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Simple and elegant white and silver chrome nail set 🤍</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qvlyjreelxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1k9xc77</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>made by me 🐝✨️</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9xc77</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1k9xamj</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Blue flowers 💙🌸</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwzf679v8lxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1k9wuf6</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>gel nails done today 💅</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9wuf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1k9vd0x</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>I have 0 experience but now im thinking about learning nails</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9vd0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1k9uqhl</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Did I lil sci-fi moment on my right hand, so I could fuck them up a bit!</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9uqhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1k9u3ta</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Second Set Ever!</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9u3ta</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1k9t7ae</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Trying press on’s</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k9t7ae</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1k92stp</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Spring Nail Inspo @nailcrush22 on tiktok</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cf4c2beafdxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1k8uffm</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Is it Good design. Can you share me your best design?</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8uffm</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Apr 30 08:12:23 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_04.xlsx
+++ b/data/collected_data/2025_05_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C494"/>
+  <dimension ref="A1:C684"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8831,6 +8831,3236 @@
         </is>
       </c>
     </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1kbb8pm</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Can i use pink biab on my builder gel nails?</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qsyvuusakxxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1kb9v3l</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Obviously fake but ok?</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb9v3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1kb8zur</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Can’t afford the salon so this is the next best thing</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjb7ts77swxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1kbagn9</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>cherry on top 🍒</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qkexp5ax9xxe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1kb907x</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Worth it?</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb907x</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1kb8tz1</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Glinda in Spring Set!</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmff3kz9qwxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1kb8dzc</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Is this set cooked?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb8dzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1kb8r7a</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Wife’s koi fish set</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqjmmumfpwxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1kb8gb7</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Beginner nail tech, what do we think?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cticgng0mwxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1kb86vh</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>✨ (Free) Online Upskilling Resources?</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mwylmf1jwxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1kb86le</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Went with a French tip</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ou1csfxxiwxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1kb7y6y</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Obsessed with color shift &amp; inspiration for nail biters</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb7y6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1kb81ha</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>New nails!!</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb81ha</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1kb7q2n</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>I Did my French tips for the first time</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axh7z7rwdwxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1kb7p7m</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>White on white!</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb7p7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1kb7m4a</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Best shape?</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb7m4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1kb53uk</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>What do I do?</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kb53uk/what_do_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1kb6o9q</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Vintage inspired</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb6o9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1kb6wjp</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Request for my 12yo daughter</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kb6wjp/request_for_my_12yo_daughter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1kb6tq5</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>I posted this nail art a few days ago, I added their missing pupils lol, I think it's much better!</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb6tq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1kb6ri3</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>First ever set of DIY acrylics</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/290tp5274wxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1kb66ii</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Another day another set</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzefkxlmyvxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1kb65dz</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Do these look like flowers or cow prints? ( I did em myself)</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb65dz</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1kb64mx</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Gel Pot Storage</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8b034at4yvxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1kb5pdt</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>These costed 40USD</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wytv7ov8uvxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1kb5jq8</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Prismatic Flower Power</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vuhdaf1nsvxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1kb5ff2</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Elegant Sparkle Nails</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t76oid9mrvxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1kb54qd</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>I don't think this is worth it</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb54qd</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1kb51pq</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Gel-X Extensions Lifting After 1.5 Weeks?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kb51pq/gelx_extensions_lifting_after_15_weeks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1kb4wr2</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hc7zu1ymvxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1kb4oc9</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Spring Nails!</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xr10qqeskvxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1kb4cij</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Dent in nail after acrylics</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hrnymbwhvxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1kb4a52</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Custom Concert Set</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb4a52</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1kb3r2x</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>I’m a man that has been told by several women I have weirdly well kept fingernails. What are your thoughts?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mczq8qkcvxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1kb3m1g</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Does anyone else paint their nails only a certain color?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kb3m1g/does_anyone_else_paint_their_nails_only_a_certain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1kb3le1</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>strengthen/lengthen nails?</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb3le1</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1kb3lnd</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>did my own nails after a 3 month break!</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dzbrdx8bvxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1kb3j8e</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Does this shape work?</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ct6f2rnavxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1kb37md</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>practicing cuticle work</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/birs47ls7vxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1kb3104</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Honest thoughts on these nails</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb3104</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1kb2y5s</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>HELP WHY?!</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fk46k4h5vxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1kb2umx</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Does this color look like a good nude for my skin tone?</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ouvpic2l4vxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1kb2kot</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Fresh paint 🩷✨</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y4khvj672vxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1kb240a</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>What color is this</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjr0oavbyuxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1kb2044</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>painted press ons</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb2044</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1kb1q4q</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>First time doing gel polish on clear press ons. Not the usual shape I would choose, I prefer shorter and more square. How do they look? I feel I may be a little blind because it feels so good to have some sort of length on my fingers.</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb1q4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1kb1oeu</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Painting over ANC?</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kb1oeu/painting_over_anc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1kb1er3</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Help! Damaged nails!</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb1er3</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1kb12os</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>new press-ons by me 🩷🙂‍↕️</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb12os</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1kb189v</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Are these good?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb189v</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1kb0wy2</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>My second time ever doing my own nails. How did I do?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb0wy2</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1kazmg5</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Ruby-zoisite inspired nails</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/joi4hkskeuxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1kazl8v</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>First Gel Mani</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kazl8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1kb0w0p</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>The timeless, the 1 &amp; only.. French manicure</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/phyg3zhaouxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1kb0l5n</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Broken nails question</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb0l5n</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1kazsix</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Making press on nails</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kazsix/making_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1kazak8</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Kiki Delivery Service Nails</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kazak8</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1kaz5ok</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>First time manicure!!</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaz5ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1kaz1qk</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Help with builder gel application</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hhwewobauxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1kayy1j</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Newest</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcpzyphk9uxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1kayvcx</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Blue and purple swirly set</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/spvhjtt19uxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1kaymce</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>New nails! Barbie Pink Cat eye and Russian manicure</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icgt11t77uxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1kaymc7</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Clean girl nails?</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaymc7</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1kayb1x</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56msi54w4uxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1kay8q7</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>nail polish q!</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kay8q7/nail_polish_q/</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1kax6q8</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>How bad did my nail tech do me?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kax6q8</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1kaxmbi</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Am I just not used to the color? Or its too much?</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaxmbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1kax196</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>My new nails</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7wszw7fvtxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1kaw9ay</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>How do I remove this safely?? It's on its last leg but just won't let go</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udzb8h1jptxe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1kawef5</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Peeled off gel polish cause I got too lazy</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kawef5/peeled_off_gel_polish_cause_i_got_too_lazy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1kaw3cj</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Think I need a better blooming gel</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0vrlalaotxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1kavz5m</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Mi animalprint 😍</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/go17y9kgntxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1kav2qi</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Beginner nail artist, struggling with press on fit. Is it okay if a little bit of my natural nail shows?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kav2qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1kaving</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>fishies</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iwzdm2r1ktxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1kavhz1</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>How long do you go between refills, and is there a point where it's better to start over?</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kavhz1/how_long_do_you_go_between_refills_and_is_there_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1kav7w8</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Rainbow nails!</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kav7w8</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1kaurho</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>How grown out do these look to you? Second picture is right after I did them</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaurho</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1katt44</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Should I be concerned?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k90o81wn7txe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1katvbv</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>In love 😍</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qwgokp448txe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1katt6m</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Eeveelution nails</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1katt6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1kato7t</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Second attempt at builder gel overlay</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kato7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1kate60</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kate60</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1katb9n</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Boho vibes</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1fupsse54txe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1kat8re</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Summer is here ☀️</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kat8re</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1kat4bt</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>All my short/natural nailed ladies - stand up!!!</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kat4bt</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1kaok1n</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>How Do I Ask For This?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdgq4tr15sxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1karp3z</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>My sweet and peaceful beach/starfish nails by @shapedbyymari</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1karp3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1kasuey</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Which color to choose for a dress with this pattern? I’d like it to be only 1 colored</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ksc27o9v0txe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1kasu3a</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2py2jtzs0txe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1kasdth</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>🔥 💅🏾🪩 what do you think?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kl3zsthxsxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1karfw7</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Spring nails 🫣🫣</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68jp8wfoqsxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1karbcl</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Benefits of having a mani similar to your nail colour (1 month growth)</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1karbcl</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1kaocpn</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>At Home Gel manicure peeling within a day</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kaocpn/at_home_gel_manicure_peeling_within_a_day/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1kalzhw</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>What do I need to do my gel nails at home?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kalzhw/what_do_i_need_to_do_my_gel_nails_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1kapprl</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Jennie from black pink inspired nails</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w8ks9rh0esxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1kaqvc6</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Kentucky Derby Nails!!</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaqvc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1kaqz2f</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>🖤</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaqz2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1kaqpew</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>My birthday nails 💕</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaqpew</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1kaqnj3</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Nezuko nails 💖</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pu7nweswksxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1kaqeag</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>My summer fruit nails 🍓</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaqeag</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1kba4vo</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>My First Holos</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kba4vo</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1kba2qb</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Surprise hit skittle</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kba2qb</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1kb8llw</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>My nails match my water bottle 💖</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb8llw</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1kb8d0u</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Somebody here posted this polish and it looked so stunning on them that I pulled it back out of my destash pile to give it a 2nd chance:</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb8d0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1kb814r</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Mooncat's Curiosity's Prey used 4 different ways: can I make it look like the swatch photo?</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb814r</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1kb7wai</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Anna Sui nail polish - barely any pigment</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9bz8v2upfwxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1kb6oqz</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Mooncat Supervillain</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6egbtsag3wxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1kb5woy</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Watching new Mooncat...</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b7sref5dvvxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1kb5rr7</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Should you dehydrate your nails before painting if they're peeling? Am I making it worse?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kb5rr7/should_you_dehydrate_your_nails_before_painting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1kb5850</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>I got my first Cracked polish and for a brief moment I thought this was part of the box design—</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxt6rhkvpvxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1kb4yoq</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>April 2025 PPU Mani</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb4yoq</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1kb4qyg</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>My Five Hundred Year Old Boyfriend! from Lurid Lacquer</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb4qyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1kb4pu6</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Show me your Ghoulish</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xs2rmy47lvxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1kb4f3v</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>inadvertently matched my work keyboard 🌈☁️</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb4f3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1kb4cya</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Wanted to show Canmake some love!!</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb4cya</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1kb43jw</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Polish Pick Up/Polished For Days question</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kb43jw/polish_pick_uppolished_for_days_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1kb40jd</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Gel Polish Suggestions</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kb40jd/gel_polish_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1kb3r62</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>perfect summer red 💋♥️🌹🎈China Glaze - Flame Boyant</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb3r62</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1kb39sr</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Space junk ⭐️💛</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb39sr</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1kb2ohw</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>What is on my nails?</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8vzkce443vxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1kb2lme</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>ILNP Enchantment 🍃🌳✨</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s0d5dx2c2vxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1kb2di4</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>So pleased with the way these came out!</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb2di4</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1kb1xk1</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Wedding Anniversary Mani</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vd3w0qgtwuxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1kb1oec</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Spring Florals</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb1oec</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1kb0hci</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Any dupes for Cirque Ethel?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5w8mfgf3luxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1kayy88</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>long lasting polish</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kayy88/long_lasting_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1kb04nz</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Castle of Cobwebs proved very popular with the minions.</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ycbl9egiuxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1kb0084</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Red &amp; gold</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb0084</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1kaz8fn</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Mmmmmmm donuts 🤤</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zdhw1j6ebuxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1kayws0</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Blue and purple swirly set</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j5dsn7yb9uxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1kayuna</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>My current hobby…</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kayuna</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1kaysjr</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>First professional manicure! Recommendations?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaysjr</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1kaym69</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>My first order from Mooncat arrived!</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5j07gkt67uxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1kaxuhs</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Rose Jelly 🥀</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaxuhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1kaxchm</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Mooncat haul came in!</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nk198igrxtxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1kaxc1t</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Worth the trip-adelic</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xlw81ablxtxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1kaxao2</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Even on sunny days, I love wearing dark nail polish 💙</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sm6fss0extxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1kawl60</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Nail art tool recs please?</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kawl60/nail_art_tool_recs_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1kaw9lq</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Out of this world sparkly! ✨ Sunken Treasure - Clionadh Cosmetics</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kybq1dukptxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1kaw4o5</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Blue Shimmer Weakness</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hkdt092kotxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1kauqpx</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>My other favorite color is this one!</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/096s62eeetxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1kaup4m</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Bees Knees Lacquer</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kaup4m/bees_knees_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1katuxp</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Nail stickers</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1katuxp/nail_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1katgt2</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>yellow butterflies ✨</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1katgt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1kat6wg</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Question about acrylic nails</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kat6wg/question_about_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1kasy70</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Still my favourite shimmery blue 💙</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dj2yzgem1txe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1kapa03</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>In love with this new set</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/al45rq0nasxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1kasmnx</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Don’t Cry Bubbles Dupe</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pyaaycbazsxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1karyl1</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Psyche Minerals</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4hwh3mzbusxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1karpwb</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Moving back to lacquer from gel - which brand to order from first?</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1karpwb/moving_back_to_lacquer_from_gel_which_brand_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1karg48</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>How about some love for Arcana Lacquer?</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ciff94qqsxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1kar5rs</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Yellow jelly flakie similar to Mooncat Powerpuff Collection</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kar5rs/yellow_jelly_flakie_similar_to_mooncat_powerpuff/</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1kar1sz</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Tennis anyone?</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1usvp30snsxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1kaqpnt</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Fish Nails</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaqpnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1kaq3t8</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>How can I make my cuticles not suck???</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaq3t8</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1kapzq5</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Dissimulation</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kapzq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1kapufh</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>From my new LynBDesigns haul! Formula is a dream 🥰</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kapufh</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1kapojl</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Gumby Green</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/no7883brdsxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1kapehd</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Cactus Makes Perfect</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kapehd</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1kaosch</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>April Manis 🌸</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaosch</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1kaogc2</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>this blue 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaogc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1kaocoj</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>the shifts are mesmerizing</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t51hansf3sxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1kanzbm</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Shimmer over magnetic</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kanzbm</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1kan7mc</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Insanely beautiful 🐻</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/alv0dq4xtrxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1kan0ds</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>IRL Colour Match - Fire Hydrant 🔥</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxewzyw7srxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1kajehg</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Help me identify these OPI minis?</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cx75jf79oqxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1kb9x0k</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Hand painted nails by me!</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb9x0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1kb9sah</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Summer nails.</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzhj5nfg1xxe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1kb8hyf</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Beginner at nails, what do we think?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znvih58imwxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1kb7obz</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>White on white 🤍</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb7obz</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1kb2r7w</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Sabrina Carpenter and other random practice nails</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rn599xzr2vxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1kb2n6l</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Kinda janky but this is my first attempt at any kind of nail art, not too bad but the charms are carrying everything lol</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyn4lw1t2vxe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1kb2594</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Disney nails!</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb2594</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1kb1uru</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>3rd set I’ve done. 1/10?</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb1uru</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1kb1c1l</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Spring nails :) All feedback welcomed</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb1c1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1kb0ner</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Torty shell w y2k inspired flaaaamesss 🔥</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb0ner</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1kayyc6</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>My nails</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kayyc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1kaydfl</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Playing with blooming gel</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaydfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1kaup48</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Little Hearts : diy 3D gel nail art</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaup48</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1katzw9</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>First Time Using 3D Charms! Pink Bow Nails!</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1katzw9</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1katq1f</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Couldn't wait to get my own stained glass set!</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52ef3ax17txe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1katjbj</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1katjbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1kat4xz</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>It's not my work, look at that design, it's beautiful.</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vfy4n7vv2txe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1kasrm1</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Did some desert spring nails</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kasrm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1kartm8</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Beautiful work today 💚💛</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kartm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1kaqx0p</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>gel on natural nails done today by me 💖</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6zyvf7tmsxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1kaqrlx</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>My birthday nails 💕</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kaqrlx</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1kapd5t</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Jelly with iridescent flakes</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kapd5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1kaodfu</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Can I use regular nail polish on gel gel nails?</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tm85leol3sxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1kakdyq</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>How do we feel about fading glitter over chrome? ✨</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6w0cz811rxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu May  1 08:12:16 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_04.xlsx
+++ b/data/collected_data/2025_05_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C684"/>
+  <dimension ref="A1:C873"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12061,6 +12061,3219 @@
         </is>
       </c>
     </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1kc30ko</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>My nails for the Coldplay concert</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cvcahg5ji4ye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1kc2s0o</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>UV pre-prepped nails</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kc2s0o/uv_preprepped_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1kc2i2p</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Cherry nails 🍒</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d36xza0zb4ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1kc2d3q</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>What can be improved?</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ielmyun6a4ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1kc1nj2</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>New nail set ideas pls!</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ed0zz8rg14ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1kc1epk</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Finding a salon that understands nail health?</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kc1epk/finding_a_salon_that_understands_nail_health/</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1kc04p5</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Side view of my nails+tutorial since some of you guys wanteddd🫣</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kc04p5</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1kc1ax6</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>For my square shape girlies</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v37cla07x3ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1kc14gp</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>My nail tech is getting better. Current set in light vs the dark. Need portable UV light to charge your polish on the go :) 🫶💅</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kc14gp</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1kc0lh8</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Did my own nails today. What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9z1his97p3ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1kc0g08</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>New set 💕</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/utcwkd1in3ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1kbzhoc</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>First set of diy gel nailsss</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbzhoc</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1kbzcgy</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>I love my nails… ❤️ this 20yo girl does nails and every time, she delivers. Also I love how my ring goes with them.</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uo7f0ctzb3ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1kbyu5y</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>LCN vs Russian Manicure</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kbyu5y/lcn_vs_russian_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1kbyl8v</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Blue as the sky</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u27qbbbb43ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1kby6wn</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>obsessed</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4g3p5pwh03ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1kbxpw0</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>How do you translate something that inspired you into nail art? Mo</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0vrknqzv2ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1kbxl32</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>first builder's gel set (customized press-ons)</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbxl32</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1kbxjwx</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>What enamel nail polish brand is best?</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kbxjwx/what_enamel_nail_polish_brand_is_best/</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1kbxho8</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Thinking about making my own press ons - where do I start?!</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kbxho8/thinking_about_making_my_own_press_ons_where_do_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1kbwova</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Are Essie "Play Date" (reg polish) and "Scavenger Hunt" (UV gel polish) the same color? I cannot find Play Date in gel form but I have seen some overlap of these two names.</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kbwova/are_essie_play_date_reg_polish_and_scavenger_hunt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1kbwee0</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Can I get some opinions on the shape please?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbwee0</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1kbvz62</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Help for gift ideas</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbvz62</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1kbvge5</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Newbie nail tech here! Just sharing the nail art sets I’ve worked on.</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6cen5mfb2ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1kbvff7</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>New Gel-X Set</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbvff7</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1kbvbz1</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>First set in 4 years</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbvbz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1kbv8me</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>My nail tech always EATS💅🏻</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbv8me</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1kbuws8</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>french + chrome 🫧</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbuws8</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1kbuv00</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>How am I doing?</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbuv00</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1kbuau5</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Where is everyone getting their press ons?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kbuau5/where_is_everyone_getting_their_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1kbt36x</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>My nailbeds burned and got swollen after i got acrylics. This has never happened before. Has anyone experienced this?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kbt36x/my_nailbeds_burned_and_got_swollen_after_i_got/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1kbtnht</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>What about the ship? They told me it's trending</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbtnht</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1kbtcra</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Elegant 🩷</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbtcra</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1kbt5jt</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Hoping I can summon some sunny weather with these 😅 I'm sick of the rain!</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bb5cgw2s1ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1kbt243</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Pink sparkle ombre</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrlwd17cr1ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1kbsxic</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Florals? For Spring?</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ealef7dbq1ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1kbsb8o</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>When your nails match your dress for your Disney trip 😍</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbsb8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1kbs8h4</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>I think this may be my new favorite set 😍</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbs8h4</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1kbs2ty</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Crooked nail</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1ykbdruj1ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1kbqyid</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Which color?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcxabplbb1ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1kbqyuc</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>thoughts on the shape? do these fit my hand well? ♥️</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbqyuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1kbqrsx</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Spring Fling!</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kbqrsx/spring_fling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1kbqqbb</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>First gel nail set ever!</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbqqbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1kbpxkg</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>My Nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgghzo2j31ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1kbq7bs</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Nail retention</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kbq7bs/nail_retention/</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1kbq5ql</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>New set ✨🧿</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5diwouu851ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1kbq3kf</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>No nail polish does dry anymore ever</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kbq3kf/no_nail_polish_does_dry_anymore_ever/</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1kbpo96</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Tricks to make them less chunky.</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbpo96</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1kbpo7h</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>I love florals for Spring time</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xtb7phl11ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1kbpetr</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Y2slay</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n324cp3lz0ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1kbotqe</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>🐆</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lklr7xa5v0ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1kbooay</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>My nail technician is tired of me being a basic bitch 😔</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbooay</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1kbon9a</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Paid $12 for these...I love a good press on!</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tc43omqst0ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1kbnszv</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Dip applied like acrylic?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kbnszv/dip_applied_like_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1kbnqvh</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>First time doing my girls nails</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbnqvh</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1kbnksy</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Bubble set 🤍✨🛁</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8sor5bxsl0ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1kbnc9k</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>First time with nails, trying to kick my biting/picking habit</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpnf5xx1k0ye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1kbn5ux</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>theme is cats n rats</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbn5ux</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1kbm4tg</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Update on my botched nails: I GOT IT FIXED!!</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37tbdtj6b0ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1kbmy0w</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>First time I get charms</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbmy0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1kbmv8i</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Did I go too crazy? 😅</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7n48unomg0ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1kbm62p</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>My first press on set!</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/555du31gb0ye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1kbm3pu</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Spring whimsy 🌸☁️</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xf98k4kya0ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1kbkln0</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Cuticle help!</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbkln0</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1kbkyb2</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>What is going on??</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kbkyb2/what_is_going_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1kblg8v</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>First timer - does this gelx look bad or is it just me?</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kblg8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1kblb3k</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>How do I stop this splitting from happening?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kblb3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1kbl9cl</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Women, how do you handle having long fake nails?</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kbl9cl/women_how_do_you_handle_having_long_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1kbljcl</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>A little addicted to lilac</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnjs8ilv60ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1kblbg1</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Spring nailsss</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kblbg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1kbl6im</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Some press-ons I made 💅</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbl6im</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1kbkqwe</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Nail popped off while on vacation what are my options?</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kbkqwe/nail_popped_off_while_on_vacation_what_are_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1kbkiml</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Double hearts because, why not!</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xuvw8df8zzxe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1kbkco3</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Why do I feel like it’s missing something?</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbkco3</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1kbkcdw</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>First Time at Nail Salon?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kbkcdw/first_time_at_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1kbjxc6</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>They look like pearls</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6rxf26zuzxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1kbjf11</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>My definition of clean girl nails</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dz51ac84rzxe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1kbjcv3</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Absolutely in love with them 🦋</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbjcv3</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1kbj4mm</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Bru I ate with this extension</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ft641l01pzxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1kbhnf0</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Cosmic baseball UV blacklight nails 👽</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbhnf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1kbfyou</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>What should I do?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbfyou</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1kbfv5t</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Why is my builder gel cracking?</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/muqyahbwzyxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1kbh080</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>I'm allergic to gels but really want to get a professional manicure done</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kbh080/im_allergic_to_gels_but_really_want_to_get_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1kbhq8k</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Genuinely the only way my nails grew back</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbhq8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1kbiobc</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Did my nails for the first time in 2 months. Still room for improvement but perfect for spring 🪷🫧</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbiobc</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1kbi150</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Love how my nails turned out🥰</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbi150</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1kbhxw1</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Did my vacation set!</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbhxw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1kbhuhw</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>I love the color red!! ❤️ different tones and always beautiful 💅</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbhuhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1kbhjis</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>End of semester reward</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvghn3sxczxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1kbgmx0</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>A nice set for my Birthday - May 1st</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbgmx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1kbgg6i</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>I need advice for at home gel removal</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbgg6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1kbfshv</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Birthday set</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbfshv</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1kbfra8</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>New Set ✨</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pfqizauxyyxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1kbems3</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Spring mani and pedi</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbems3</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1kbemfe</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Orange, red aura, &amp; chrome</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbemfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1kbe9dh</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Constructive criticism</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lybr1eq7lyxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1kbe6iz</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Constructive criticism</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nk3z3zqfkyxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1kbe5y9</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Constructive criticism</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5t4dxn9kyxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1kbdett</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>something fun finally!</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43zyjne7cyxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1kbd3o8</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>How can I improve shape and thickness?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbd3o8</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1kc3ikg</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>NOOOOO HELP!</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kc3ikg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1kc3047</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Blue shimmer comparison and a secret.</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kc3047</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1kc1z8v</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Found my perfect nude?</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qlyge6zc54ye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1kc1fwi</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>accidental mardi gras vibes with my HHC swatch mani!</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kc1fwi</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1kc0yb7</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Matching my nails to my knitting</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ns1g3u5t3ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1kc0166</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>First Clionadh Polishes!</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kc0166</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1kbzrum</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>April Manis 💜</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbzrum</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1kbzgfi</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>ID this peachy color</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/esum90w3d3ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1kbywzb</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Experimented with a magnetic powder</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1dhwi4hi73ye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1kby76d</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>IIL Mooncat’s Maelstrom, what else will I like?</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kby76d/iil_mooncats_maelstrom_what_else_will_i_like/</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1kby5uz</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Cirque pyro</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kby5uz/cirque_pyro/</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1kby5cw</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>I organized my collection and put it out to be seen and enjoyed (by me)</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kby5cw</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1kbxzni</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Treachery in the Blue + Flower Child</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbxzni</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1kbxb2w</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>I guess after 3.5 weeks it’s time to let her go :’)</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbxb2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1kbwodt</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Are Essie "Play Date" (reg polish) and "Scavenger Hunt" (UV gel polish) the same color? I cannot find Play Date in gel form but I have seen some overlap of these two names.</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kbwodt/are_essie_play_date_reg_polish_and_scavenger_hunt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1kbw7x1</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>New fav combo?</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbw7x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1kbe25g</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Best base and top coat (regular polish)?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kbe25g/best_base_and_top_coat_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1kbuyvd</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Multichrome and Crackle</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbuyvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1kbufnq</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>like air, I’ll rise ✨</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbufnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1kbu86v</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>peachy confection for spring</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbu86v</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1kbu74y</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Green Goodness!</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v29dil3q02ye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1kbtn8b</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Mooncat and BKL</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbtn8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1kbt4pd</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>LA Colors SEASHELL GLAM</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9b71h6nvr1ye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1kbsr1g</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Cock a doodle Doom may be one of my top favorite nail polishes. I feel like photos don’t do enough justice. It’s SO beautiful!!</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wai4iycwo1ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1kbscr5</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Zoya Flash BOGO</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dscr2hexl1ye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1kbsabg</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Inspo: gardening in Oklahoma (IYKYK)</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1pyk73fl1ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1kbs4h8</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Transcience</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbs4h8</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1kbrui6</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Removal Method Tips</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kbrui6/removal_method_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1kbremg</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Fables and Folklore - February 2025 PPU, Decant Edition</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbremg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1kbr4xt</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>In my crone era</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbr4xt</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1kbr4ts</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>My dream pink: Tropical Gasflame by Alchemy Lacquer</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbr4ts</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1kbqzoj</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Help me find a similar magnet!</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbqzoj</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1kbpyx3</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Tropical Gasflame by Alchemy Lacquer is ✨that pink✨</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbpyx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1kbpqd3</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Where are all my neons at?</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbpqd3</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1kbppj8</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Weird dip near the cuticle of my nails</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbppj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1kbpddj</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>NOOOOOOO😔💔</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbpddj</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1kbp5e1</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Can folks please post their swatches/manicures of “Eternal Glow” by Polished For Days? (Nail image not mine)</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqkoxkhlx0ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1kbp3h0</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>ILNP Deep Dive + Stickers</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbp3h0</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1kbovtk</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>April Manis ☔️</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbovtk</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1kboac7</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>ILNP Looking Up</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4d2z4o3r0ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1kbn8y3</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>I got my first “Ooo did you get your nails done??” Today!!!</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yurei0bcj0ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1kbn362</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Best jellies/crellies I can get at the drugstore?</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kbn362/best_jelliescrellies_i_can_get_at_the_drugstore/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1kbmxl6</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Matte metallics. That is all.</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0u9fr54h0ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1kbmmb6</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Terraria Party Girl</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbmmb6</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1kbmffc</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Holo Taco - Toe Beans 🐾</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qs8ghpcd0ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1kbm242</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Storage Question</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kbm242/storage_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1kblx5t</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>New Mani for me</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yhrse3am90ye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1kbl9xl</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>LA Colors Meteorite over black</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbl9xl</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1kbkxkk</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>This has to be their best seller</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fr8m829d20ye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1kbkutv</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>What i asked for vs what i got (and a bonus slide of gel polish on my fucking skin)</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbkutv</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1kbki0x</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>My partners nails after I painted them</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0c920m7zzxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1kbk8nf</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>✨Fancy Fingers✨Tom Ford</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnrn2pw9xzxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1kbjyzf</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Bright neon blue!</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbjyzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1kbjrx4</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>LA Colors HORIZON</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wk6jy7cvtzxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1kbjq11</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Help I tried out thermal and now i cant stop playing with the effect xD</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbjq11</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1kbjcnj</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>I finally did a good mani last night and I’m proud of myself.</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbjcnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1kbjcm3</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Top Fav Purple</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbjcm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1kbjbht</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>It’s finally here! Magic Frog by Lumen (videos in comments and please ignore the ding on my pinky)</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbjbht</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1kbizzu</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>horseshoe magnets are magic</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cfnkg2q2ozxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1kbiyhl</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>looks different in every lighting</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbiyhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1kbim4i</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Topcoat help</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tx11mdkalzxe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1kbhwrs</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Penelope Luz - Magical Place</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ge23gj0wfzxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1kbhv5b</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Heart magnet (cat eye polish)</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpjqnnvifzxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1kbhhw4</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>why does my middle fingernail have those white spots</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekin1pvlczxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1kbh9wm</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>KBShimmer polish thinner compatible with thermals?</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kbh9wm/kbshimmer_polish_thinner_compatible_with_thermals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1kbh6df</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Cost effective oil for warm oil baths?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kbh6df/cost_effective_oil_for_warm_oil_baths/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1kbgkwv</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Tie-dye vibes</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbgkwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1kbfag0</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>All my April Manicures</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbfag0</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1kbeoyt</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>My husband said he needed the round magnet for a project, this is how he got it</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1taj71gpyxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1kbdggc</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Any New Zealand Laqueristas keen to share ILNP shipping?</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kbdggc/any_new_zealand_laqueristas_keen_to_share_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1kb5rk4</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Alchemy Lacquer haul 🩷 the packaging is soo cute</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kb5rk4</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1kc3fj4</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Trying new stuff</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kc3fj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1kc0whe</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>cherry red nails! 🍒</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zub637tks3ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1kc0dy6</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>LF Nail Art Tutorials</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kc0dy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1kc0cst</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Devil nails 😈🍒</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kc0cst</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1kbya40</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>What do we think</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbya40</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1kbvc2h</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Hi, I’m a newbie nail tech. These are my nail art sets I’ve done to see what I can do and practice expanding my capabilities.</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4lrge4ea2ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1kbtjkx</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>UK based nail people</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kbtjkx/uk_based_nail_people/</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1kbs0pd</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>My nail tech is great!</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9rvrawej1ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1kbr7tf</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Naming this set acid pixie 💚</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbr7tf</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1kbqz32</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>attempted a very small slay</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbqz32</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1kbqd8r</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>como me quedaron ?</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtvj9ydp61ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1kbo3uj</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>💜☁️</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1k7sn9pp0ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1kbn5br</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>cow nails- udder included 😁</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbn5br</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1kbm0uw</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>rubber gel made today by me 🫠</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lsb2dltea0ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1kbkmop</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>would something like this be possible without airbrushing</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/na5ww2b600ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1kbeu20</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Winnie-the-Pooh</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbeu20</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1kbdovb</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>How to Ombré Rainbow glitter nails?</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kbdovb</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1kbbzhs</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>💙💙aura</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ln9yh3iduxxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri May  2 08:12:08 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_04.xlsx
+++ b/data/collected_data/2025_05_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C873"/>
+  <dimension ref="A1:C1037"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15274,6 +15274,2794 @@
         </is>
       </c>
     </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1kcv00k</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>best gel base and top coat?</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kcv00k/best_gel_base_and_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1kctui7</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Got to love French tips.</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oh7brv7n6bye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1kcsxhs</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Some of my favorite sets (some were boomerangs sry if they’re blurry😭)</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcsxhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1kcso7f</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Are these bad?</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcso7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1kco54r</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Can someone explain nail salons to me?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsk1yx1lk9ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1kcsczj</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>What shape are my nails?</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7e6nl8oipaye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1kcrhc2</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Press ons from dollar tree</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7ndrcj7gaye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1kcre81</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>On a budget press on nails</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sp27fmcqeaye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1kcmtn7</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>I’m going insane, I want to be able to wear press ons but they keep popping off, please help!</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcmtn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1kcpvil</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Can someone please Amazon link me to a neutral gel nail polish for dark skin ? Picture included</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0914qwnq0aye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1kcqu2n</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>What nail color would look best with my engagement ring?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmwqvluw9aye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1kcq1kj</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Male Art Pedicure</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcq1kj</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1kcqehr</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Cowboy Carter Nails</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcqehr</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1kcq85a</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Feel like im sacrificing quality to save a few bucks</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kcq85a/feel_like_im_sacrificing_quality_to_save_a_few/</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1kcp6k6</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>nails with cats 💅🖤</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ciz5xje8u9ye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1kcp49n</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Who can notice the mistake I did? 🥲 🤣🥲</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b5vn4j8nt9ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1kcov88</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>What are good nail lacquer top coats and base coats?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kcov88/what_are_good_nail_lacquer_top_coats_and_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1kcop27</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Pretty in pink!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcop27</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1kcoaul</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>my favorite set i’ve ever gotten</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzzocks1m9ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1kco4ws</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Gave my nail tech creative freedom</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kco4ws</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1kcnqjw</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Celestial Aura Nails</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcnqjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1kcnogq</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Nail Cost</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcnogq</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1kcnodz</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>New set, feels slightly incomplete?</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcnodz</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1kcmmxa</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Wondering if there’s a answer to my question¿</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kcmmxa/wondering_if_theres_a_answer_to_my_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1kcmhf1</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Evolution of my acrylic</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gt8w16t169ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1kcm5gi</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>i love french chrome 🩵💙</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8mfl3bc39ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1kck6kz</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>what kind of nails work best on chubby fingers?</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0bcjehln8ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1kck60f</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>I want tips/extensions but don’t like dip or acrylic. Do I have other options??</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kck60f/i_want_tipsextensions_but_dont_like_dip_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1kchr29</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>First time getting short square</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kchr29</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1kciph2</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Recently developed an allergy</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/si6wnqafc8ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1kcj9k0</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>First attempt at extending nails using extend gel and builder gel. Constructive criticism appreciated!</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcj9k0</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1kci3ru</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Yellow 💛🌞</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kci3ru</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1kci11i</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>First time full polygel set and I’m never going back to a builder.</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rlncdkic78ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1kchyuu</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Cutting &amp; Shaping</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5hfvdjo68ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1kchvac</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>just did my first nude set!</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1f7pvc568ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1kchtz8</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Slay or nay?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5iq4g0kv58ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1kch2fy</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>First time with builder gel</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kch2fy</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1kcg6zx</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>My friend has been doing my nails..</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kcg6zx/my_friend_has_been_doing_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1kcg58w</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Nail strengthener - not gel or dip</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kcg58w/nail_strengthener_not_gel_or_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1kcf7sq</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Jewels and jungle</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcf7sq</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1kcemn5</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Got my nails done yesterday inspired by a book</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcemn5</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1kcgdax</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Should i go back to this nail artist?</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcgdax</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1kcfx7e</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Press on question</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qyv0r8fhr7ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1kcfsy4</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>My niece said it looks like fairyland</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnudbx2mq7ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1kcf48u</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Cheetah Hello Kitty freestyle</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcf48u</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1kcf2l7</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>My fresh Powerpuff Girl nails :)</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcf2l7</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1kcezhn</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Pink press ons I did xx</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/be07lyekk7ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1kcevnc</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Cadillacquer - Everything Will Change</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qaaunwisj7ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1kcdyvx</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Matched my nails to my crocs</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nj2x9sv4d7ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1kcdrhg</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kcdrhg/question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1kcdds2</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>My First Time💅!</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6w6u2zms87ye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1kcddv2</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Drop Chrome/pearl Powder Recommendations!</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0snzpldu87ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1kcckhl</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Design choice?</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcckhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1kccxlt</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>My nail artist slaps!</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qojyh8dj57ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1kccldg</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Is it the polish or my natural nails??</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kccldg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1kcakwj</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>My press ons are splitting in half :(</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kcakwj/my_press_ons_are_splitting_in_half/</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1kc9rak</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Sore nail beds after BIAB - how can I prevent further damage?</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kc9rak/sore_nail_beds_after_biab_how_can_i_prevent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1kc8tcd</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>SOS - only it’s my nails!</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zmevmqla6ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1kc82xl</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Fake nail cuticle rash?</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kc82xl/fake_nail_cuticle_rash/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1kc4vnw</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>How do I get my nails to stop chipping?</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kc4vnw</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1kcboto</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Obsessed with pierced nude nails!</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/esxv6x9fw6ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1kcatqs</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>My simple spring set ☀️</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7758w77q6ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1kcaplk</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>after a hiatus</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcaplk</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1kc9qmf</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Long and colourful!</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/njiw4bpuh6ye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1kc9cn1</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Did my first gel nail set:)</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gwjrd22ve6ye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1kc7l58</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>HELP 😭😭</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kc7l58/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1kc6sph</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>These are fake nails I bought from shein and made them myself at home. What do you think?</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kc6sph</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1kc6cv5</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Had to visit my favorite nail tech in Japan</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnnuyrq5o5ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1kc687n</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>A friend said I don’t do pink enough, so I went with DND gel ‘Hibiscus Platinum’</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kc687n</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1kc5ypf</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>These are the longest nails i've ever had 😍</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74r9ks1zj5ye1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1kc4yfi</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Graduation nails</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kc4yfi/graduation_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1kc49s7</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Work nails go hard when everyone is noticing them 👼</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kc49s7</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1kc44vo</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Nails over the years</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kc44vo</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1kc3yf7</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Yellow with black splatter and gold foil</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kc3yf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1kcv5fb</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>OPI Make 'em Jelly</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kcv5fb/opi_make_em_jelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1kcv599</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Root of All Evil</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcv599</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1kcum9u</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>An update on the nails</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7930vz6gbye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1kcu7mo</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Roe, Roe, Roe Your Vote</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcu7mo</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1kct9qx</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Big News Everyone!</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kct9qx</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1kcrnq1</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Acetone to-go?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugh8u2g2iaye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1kcrnkg</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Lylah's Jewel Beetle, RIP Lylah</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcrnkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1kcr8ir</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Velvet nails: Sj3 velveteen magnet or 30 lb horseshoe?</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcr8ir</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1kcr379</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Vampire’s Desire</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcr379</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1kcqx5g</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Lurker turned poster</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcqx5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1kcqwi9</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Have you stared at your nails today?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kcqwi9/have_you_stared_at_your_nails_today/</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1kcqjfd</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Looking for candy style polish to match</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcqjfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1kcpk9o</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>I can never do a mani without glitter ✨</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4alwgo4ux9ye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1kcpi8g</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>What are your pet peeves about painting your nails?</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kcpi8g/what_are_your_pet_peeves_about_painting_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1kcp27z</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Am I crazy or do these nails make me look sick</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8pm4714t9ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1kcoiq3</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Any good dollar store topcoats by chance?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kcoiq3/any_good_dollar_store_topcoats_by_chance/</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1kcogsn</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>“Let’s share a Paopu fruit, because there’s nobody else I’d rather enjoy a sea-salt ice cream with"</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcogsn</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1kco2z9</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Cotton candy skies</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kco2z9</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1kcns3z</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Celestial Aura Nails</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcns3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1kcnl4k</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Getting my sparkle fix while I wait for norpsilocin ✨</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d1mhxsflf9ye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1kcnddb</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Who is the best example for the best long red nails?</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kcnddb/who_is_the_best_example_for_the_best_long_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1kcmi4n</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Guess what Pokemon this fluid art mani is based on! Winner gets bragging rights. Hint: it’s NOT Sylveon.</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcmi4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1kcmguh</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>The best mani lighting available to me is this mildly dismal lighting at the gym</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a61f056x59ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1kcmga2</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Velvet nails! Been super overcast, so this was the best I could get. Used a 30lb. horseshoe magnet. ILNP Lightwave.</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yagsz16s59ye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1kck4hw</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Death Star!</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzrb0si7n8ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1kcm5if</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Help me make a flower petal topper!</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kcm5if/help_me_make_a_flower_petal_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1kcm22q</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Fancy Gloss- Pastel Pink Mix [Topper]</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcm22q</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1kclgz3</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>What is with this color?</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fja6tmrx8ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1kcky0q</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Test running the mani I wanna wear for trip I’ll likely be proposed to during 💍💅Feedback appreciated!</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xb5ddikt8ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1kckxyn</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Looking for the perfect "blue"-red</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ww0l9b50t8ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1kcjw2o</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Pink upside down french tips</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcjw2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1kcjue8</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>velvet magnetic, holo sparkle AND iridescent shimmer? yes please!</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nqp9isz0l8ye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1kcjcmf</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>How often is too often?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kcjcmf/how_often_is_too_often/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1kcisl3</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Vacation Manicure</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcisl3</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1kcin9b</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Matching with My Fountain Pen</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcin9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1kciein</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Spring Sunshine</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kciein</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1kci02z</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>I don’t know about her</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvs903n478ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1kcfy86</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Reviews for Le Mini Macaron Soft Gel Tips</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kcfy86/reviews_for_le_mini_macaron_soft_gel_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1kcft3c</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Finally, a blur that this brown girl LOVES</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcft3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1kcfdvd</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Moon kitten forever</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcfdvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1kcf8h5</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>obsessed with this polish</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcf8h5</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1kcf7em</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>in my magnetic era</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bxb1frf7m7ye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1kcf3m5</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Gaining Length ☀️</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcf3m5</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1kcex2p</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Does anyone know a nail polish with this colour?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzhzq3u2k7ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1kcevzt</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Cadillacquer - Everything Will Change</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9wzlvwruj7ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1kcer0z</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Polish ideas for 30th birthday?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcer0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1kceiye</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>How do you feel about jelly polish?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kceiye/how_do_you_feel_about_jelly_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1kcee88</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>💜🩵Tropical Sparkle🩵💜</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcee88</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1kcedzy</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Mooncat's Sagebrush really is that bitch</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcedzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1kcd1in</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>whats your painting routine?</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4qgrcvc67ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1kccxc0</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>What to do?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21bwiikh57ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1kccmnt</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>How to keep polish from chipping?</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swu2nugb27ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1kccfk4</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Got got by Lumen’s Glass Jellyfish</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kccfk4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1kcc5lx</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Kbshimmer Comparison Request</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kcc5lx/kbshimmer_comparison_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1kcbzar</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Is there a color family you like now but used to avoid?</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kcbzar/is_there_a_color_family_you_like_now_but_used_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1kcaxgm</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Curiosity’s win</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcaxgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1kcaaoq</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Cosmic Cowboy</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcaaoq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1kca7z3</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>8yr old said I have booger nails 🙃</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kca7z3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1kc9vpf</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Alternatives for cuticle oil?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kc9vpf/alternatives_for_cuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1kc9pq3</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Ava by ILNP</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kc9pq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1kc8yni</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Sparkle Overload! ✨️</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hrifsx1sb6ye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1kc8cin</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Which nails would go harder on my character</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gd9az0q766ye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1kc8826</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Spring highlights 🦋</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3ysszqn56ye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1kc6dlu</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Had to visit my favorite nail tech in Japan</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnnuyrq5o5ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1kc51ne</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kc51ne/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1kc4kyq</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>ILNP Starlight</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbh7pqvb35ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1kbxwhr</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Favorite orange/copper polishes?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kbxwhr/favorite_orangecopper_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1kby58d</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>need help with seche vite</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g5kl4fvyz2ye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1kct9e4</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>how do i make french tips even?</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kct9e4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1kcs35t</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Simple nails are always the best! Does anyone agrees with me?</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kcs35t/simple_nails_are_always_the_best_does_anyone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1kcqu2p</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>May pole themed hand painted press ons</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3toyqdip9aye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1kcqapw</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Boyfriend tax</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcqapw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1kcq77h</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Fish Market!</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvfsmbft3aye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1kcoppc</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Pretty in pink!</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcoppc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1kco0ov</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Jiji nails! 🐈‍⬛🐾</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mlvsurgj9ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1kcnxpf</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Made a set of nails inspired by Rafayel from Love and Deepspace ♡</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcnxpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1kcnr3i</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Celestial Aura Nails</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcnr3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1kcmfjr</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Moziac shell tips 🩵 and chrome!</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcmfjr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1kckbrf</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Another day another set</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kckbrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1kcjaev</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>que tal me quedo este trabajo que le hice a mi prima ?</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmfn3djog8ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1kcgl1v</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Buggy 3D nail art I did</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqfhlvyew7ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1kcgjao</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Tips on how to make your polish not so streaky? Jo</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rz8no2k1w7ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1kcf7pv</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Mrs Frizzle nail art idea</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nw65oo2am7ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1kcf2xh</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Jewels and jungle</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcf2xh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1kcetzg</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>New to press ons - how do you handle sizing?</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kcetzg/new_to_press_ons_how_do_you_handle_sizing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1kceikp</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>One of my favorites</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kceikp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1kce6qq</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Rhinestone take over!</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kce6qq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1kcd5sk</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>It's been a minute. But here's some glitter ✨</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypkff8w777ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1kcd55m</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Wedding nail art ideas?</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcd55m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1kca976</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Diseño hecho por mi hoy , naturales ✨️</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzifb9sul6ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat May  3 08:10:21 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_04.xlsx
+++ b/data/collected_data/2025_05_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1037"/>
+  <dimension ref="A1:C1244"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18062,6 +18062,3525 @@
         </is>
       </c>
     </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1kdno0a</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>I’ll be getting my first Russian manicure tomorrow!</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kdno0a/ill_be_getting_my_first_russian_manicure_tomorrow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1kdmxya</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>I am so happy with how well my nail tech did this time around 🤩</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thdon8wvmiye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1kdjzf8</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>librarian tips and tricks?</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kdjzf8/librarian_tips_and_tricks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1kdmmqj</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>I wanted someting simple and spring vibes💙</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jo908y76jiye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1kdmfv3</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Filing after polish?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kdmfv3/filing_after_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1kdm8g8</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdm8g8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1kdjjeh</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Acrylics newbie</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kdjjeh/acrylics_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1kdihg1</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Obsessed with chrome</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/reatyd23ahye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1kdlz2r</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>pink is in session 💗💗</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4o6wb4j9biye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1kdkeii</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>my nails are too long</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdkeii</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1kdkmq6</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Accidentally matched my phone case</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdkmq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1kdloe2</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Simple but cute !</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drad3kvp7iye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1kdlkeg</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>my tech ate w this one</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tmpndgjg6iye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1kdlhow</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Floral scalloped frenchies</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdlhow</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1kdl9pg</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Update to choosing my best nail shape!</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3erif0zu2iye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1kdl8r6</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Birthday nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nyhuy0fq2iye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1kdkczc</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>this weeks nails</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdkczc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1kdkc21</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Glittered nail obsession!</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdkc21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1kdk2ye</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>What’s the best color for formal occasions?</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kdk2ye/whats_the_best_color_for_formal_occasions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1kdjz85</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>I miss acrylics</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdjz85</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1kdjs74</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>My Summer gel jelly nails</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdjs74</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1kdj4xx</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>My Favorite set so far. What you guys think ?</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q30k8kpkghye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1kdj17c</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Perfect nude nails ☺️</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4te6tfkfhye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1kdizi5</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Nail tech in NYC</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kdizi5/nail_tech_in_nyc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1kdif4s</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6vzxy8g9hye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1kdicz9</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>White nail polish</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kdicz9/white_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1kdiaec</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Wanted to share my wedding nails</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdiaec</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1kdi2im</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Am I going to just have to cut my nail short?</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0h1x6wy5hye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1kdhwia</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Cat eye French</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8h5q5v6e4hye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1kdhtf3</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>I'm back baby!</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdhtf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1kdhsea</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Chrome is my favorite 💖✨️</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdhsea</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1kdh5uu</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>🦋🍃</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n09m5rz6xgye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1kdh5t4</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Sunshine in the Garden</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wolyacl6xgye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1kdgan4</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Top coat on 3d nail art</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kdgan4/top_coat_on_3d_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1kdfury</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Some recent sets of mine.</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdfury</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1kdgw4v</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Hated my nails for two weeks but now I’m in loveeeee</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdgw4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1kdgmct</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Do you like this new design?💅</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etd7mdx6sgye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1kdgjux</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Fresh set!✨</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdgjux</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1kdgjud</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>i got my nails done for my first prom</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdgjud</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1kdfsyx</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>First time doing pink!! I did a different shade for my toes.</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdfsyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1kdfsig</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Nail shape help!</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdfsig</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1kdfk0c</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Would this be an ok formula?</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kdfk0c/would_this_be_an_ok_formula/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1kdeqcq</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Should I get these fixed?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pw0r6j0hbgye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1kdbiu5</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Which one should I do??</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdbiu5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1kdfn24</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Sturdy andReusable nail glue for stick on nails</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kdfn24/sturdy_andreusable_nail_glue_for_stick_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1kdfiwa</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Just got them done ✨</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdfiwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1kdf552</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>My nails matched a Cherry</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q1jq6hgzegye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1kdf4q6</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Kept it simple 👀💅</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ol7da8wegye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1kdeukb</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>First try at marbling, water using modeling gel, and dragon skin/eye (also using the modeling gel)</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdeukb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1kdetpf</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Haven’t had nails in years but finally feeling like myself again!</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdetpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1kdetjn</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>I made Littlest Pet Shop nails!🌈✨</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdetjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1kdduvd</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Purple Gemstone Nails 💜</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdduvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1kddsfe</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Beginner Gel Nails</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnv6y3cn3gye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1kddpq9</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>My nail tech showed me so much love after I lived like a cavewoman for the last eight months due to pregnancy. Now I can’t stop staring at my hands!</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mj4bnmb13gye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1kddf2k</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Can/should I try to file these ANC nails?</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ndiqus7o0gye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1kd1k1f</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>I was injured 15 years ago and it still grows like this ! What do i do</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rszj10pmjdye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1kddfqn</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>My first post here! My nails ready for the premiere of my favorite movie!</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kddfqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1kdd7tz</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>What could I charge for press ons like these?</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdd7tz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1kdcyps</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>I asked for something I’ve not seen before and I think my nail tech nailed it</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncl3kgv4xfye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1kdcwtx</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Russian manicures are unbeatable</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kdcwtx/russian_manicures_are_unbeatable/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1kdcmff</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Violet for May</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdcmff</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1kdcc30</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>tiny floral nails</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35f25n37sfye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1kdc86q</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Dreaming of the beach</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7mb1lm5crfye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1kdc7nz</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Opinions on dip powder nails?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kdc7nz/opinions_on_dip_powder_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1kdbo9j</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Wanted a natural color</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9b5ro0tmfye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1kdbf9q</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Best UV/LED lamp non professionals can buy?</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kdbf9q/best_uvled_lamp_non_professionals_can_buy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1kdbc50</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Could I use this with a UV lamp for a gel manicure?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgpqby5ikfye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1kdb2mo</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>french tip 🌸🎀🌷</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdb2mo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1kdb077</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Hard gel manicure</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scbrcsuyhfye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1kdayk0</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Y2K goth</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/waraax9nhfye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1kd8qki</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Need a new nail shape</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fl1fh0ju0fye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1kda4zl</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>My nails are soooo ug*y please help me</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kda4zl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1kd913u</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y59pha303fye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1kd73h7</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Vaporware nails</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd73h7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1kd8jv7</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>30 Days of nails - Day 1 - Psychedelic Swirls 🌈🍭</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lytccsr3zeye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1kd8f78</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>New to acrylics, how can I communicate with tech better?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd8f78</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1kd7yed</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>🐌💅</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x31chnjtueye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1kd6zvr</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Got my nails done today~</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxr18cuqneye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1kd6xjr</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>first time with 3D nails!!</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkln48t9neye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1kd6787</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>how can i fix my nail?</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd6787</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1kd5zig</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Are these worth it?</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/htyu0afcgeye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1kd5kwn</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>How do I grow my nails out when my free edge keeps flaking and breaking?</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cb9uh7dbdeye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1kd5pyr</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>How much would you pay for these press on nails?</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/htzqr08beeye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1kd5pfq</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Here fishy fishy</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd5pfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1kd5iz3</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>If I am getting a builder gel manicure and I accidently broke 2 nails, is it okay to ask the tech to add length to those so I don't have to cut my natural nails?</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kd5iz3/if_i_am_getting_a_builder_gel_manicure_and_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1kctw1f</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Mexico trip inspired</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kctw1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1kcx6wv</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>angel wings feat. charms and lace background</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcx6wv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1kd528j</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Love how they turned out &amp; love the colors</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd528j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1kd4rah</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Working on my frenchies :)</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd4rah</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1kd4ojz</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Trying a new style</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd4ojz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1kd3mfn</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>My favorite set so far! I’m obsessed with these!!</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ifun314yydye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1kd3lai</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Did my French manicure come out bad?</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0iiol7qydye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1kd2w7k</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Is this bad, and will it go away?</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2my6ruptdye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1kd0el8</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Help me choose a good regular nail polish!</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kd0el8/help_me_choose_a_good_regular_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1kd2qks</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>What should I have done next time I go to the nail salon? I liked what I had done recently here.</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrbi6azjsdye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1kd0wew</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>I've taken a break from acrylics for about 6 months, and noticed these red dots recently, is it from the acrylics and just slow to show?</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd0wew</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1kd2bec</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>To chrome or not to chrome…</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/puuwiwoepdye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1kd1zq3</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>New set for my birthday!</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mw6fvziymdye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1kd1xgl</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Rainbow chrome</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fjvwe79gmdye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1kd1vmm</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Louboutin Vibes👠💅</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd1vmm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1kdn7sy</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>The galaxy nails of my dreams🪐</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t9d7hv35qiye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1kdn6ii</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Hit the Bottle peel off basecoat - PPU</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pw7ky2rpiye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1kdm564</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Queen of Rot will be Back 🥳</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjsghjd1diye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1kdlwhh</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Newbie to indies - what's everyone's rec for a true neon yellow?</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2ze6jveaiye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1kdkfi7</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>"Ooohhh" Cracked 💜</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdkfi7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1kdk9zb</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Clean nails obsession</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdk9zb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1kdk9h4</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>I got to try my first thermal and I can’t stop staring!!</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdk9h4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1kdj5cg</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Oops I duped it again 🎶 What's a polish you've accidentally duped with something you already own?</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kdj5cg/oops_i_duped_it_again_whats_a_polish_youve/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1kdj3vf</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Deep Blues and Golden Hues</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdj3vf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1kditdf</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>He is Coming 🦇🕯️</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yiygmzqddhye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1kdiqxx</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>I think I might have found the perfect feminine rage polish</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/re4qhvtpchye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1kdhvqa</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>wonky nail shape?</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdhvqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1kdh94o</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Sunshine in the Garden</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1621rc13ygye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1kdgz6d</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Can you post your ILNP Cygnus Loop?</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kdgz6d/can_you_post_your_ilnp_cygnus_loop/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1kdgik5</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>First-time poster!</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxaxqnn8rgye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1kdgeqp</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Suggestions for big fat flakies??</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2vous39qgye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1kdfelm</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>March and April recap!</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdfelm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1kdegpi</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Peel off glitter topcoat</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kdegpi/peel_off_glitter_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1kddtoh</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Gel polish lamp question</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://a.co/d/egBh0XN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1kddjsw</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Experimenting with neon powder, didnt expect much but damn these colors POP 🌈✨️!</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kddjsw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1kddh7j</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>$50 on fb marketplace - would you bite??</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kddh7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1kddf4t</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Any advice for doing french tips with shaky hands?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kddf4t/any_advice_for_doing_french_tips_with_shaky_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1kddduh</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>It's finally a bank holiday weekend (UK) where I'm not working!</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyy5xrfc0gye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1kdd838</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>banquet of doom!</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdd838</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1kdd1wl</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Essie Gel Couture Top Coat Lifting</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bc5pokotxfye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1kdcd6s</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Violet for May</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdcd6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1kdccyr</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>the hype is real 💙</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdccyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1kdcb3f</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Okay okay okay I GET it now 🍄🌈✨</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdcb3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1kdbypt</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Coffee Storm and Furb’s the Word</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2awi0jgapfye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1kdbxfx</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Red Eyed Lacquer Swatches</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdbxfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1kdblr2</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Calling all Mermaids - You are welcome in advance!</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdblr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1kdbgng</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Reshaping crooked nails</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdbgng</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1kdb4pp</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Pull it Together 💚</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdb4pp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1kda5zj</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>dupe for madam glam’s hardcore please!</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kda5zj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1kda5jo</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Vice 2025</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kda5jo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1kda3ls</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>did i grow my nails out to provide better scritches for my cat? it’s possible</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzyyw195bfye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1kda2ed</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Ghost Ray✨👻✨</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v2lz2ewtafye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1kcmyw7</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Blue gradient</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rwjjxx6a9ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1kd1fzj</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Candles &amp; Chaos</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kd1fzj/candles_chaos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1kd9m8c</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Powerpuff gradient</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd9m8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1kd9377</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Luminary from Alchemy Lacquers ☀️🤩</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gmnylure3fye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1kd8v7t</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>I’m obsessed 🌡️🥰</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd8v7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1kd8prr</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Love Ilnp Polishes</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd8prr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1kd8gkj</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>U Is for You and Me</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd8gkj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1kd8g32</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Finally used my I magnet correctly thanks to this chat!</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3kephqskyeye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1kd85tx</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>does anyone have any polish recommendations similar to this beautiful red?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6wfig0eweye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1kd84tc</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>“Spirit of Halloween” for spring? Sure!</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd84tc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1kd80hj</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Pretty rainbows 🌈 😻</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0dwdmw8veye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1kd7tu8</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Nail Art Progress-cat abduction skittle set</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd7tu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1kd7mrx</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Ghoulish</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd7mrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1kd6x01</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Pretty Pretty Princess nails!</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0woufkj5neye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1kd6w4e</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Anyone else have uneven nail growth?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vjxax7zmeye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1kd5z1a</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Skittle from my haul! Comparison</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd5z1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1kd4wri</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Nails too weak for rubber base?</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wuauejb8eye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1kd4s1m</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>polish changes lives (nail beds)</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd4s1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1kd4fqj</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Love the color, love the flakies, but the formula on this one... meh</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fsmflcvv4eye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1kd4c21</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>cracked polish shut the front door</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd4c21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1kd4ab8</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>a controversial skittle</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd4ab8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1kd3iu9</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Help me find dupes for May PPU!</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd3iu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1kd3cow</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Mooncat - Twilight Sonata</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/49zyff8zwdye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1kd2yf9</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Plumpest top coat you've tried??? Pic for attention lol</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd2yf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1kd2y88</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Advice</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rz70qd63udye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1kd1t8x</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Rose gold flakes</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd1t8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1kd19oc</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Dark &amp; Twisted Lacquer Moonlight Cruising</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd19oc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1kd191z</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Waltz of the Flowers 😍✨</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tze3sd7hdye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1kd10zj</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Tomato Girl Summer 🍅</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd10zj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1kd0ye6</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>The blue shimmer in It’s Going Tibia Okay 🫠</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzi5xalsedye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1kd0p3g</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>🤍💙Piet Mondrian❤️💛</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd0p3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1kd0mij</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Any allergy safe press ons at Target?</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bycrfcq3cdye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1kczzlo</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>You never think it'll happen to you</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfcwi8zd6dye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1kczxrm</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Immediately knew I had to put this one on, and now I can't stop doing this...</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/txmjvmp26dye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1kczixi</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>“What’s That In The Mustard?” from Broken Pixel Polish</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kczixi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1kcz5kr</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>When the last minute cart addition ends up being your fav</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcz5kr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1kcz273</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>BIAB nails and piano</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kcz273/biab_nails_and_piano/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1kcyv76</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Crystal Knockout</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcyv76</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1kcypd2</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Blood Moon</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcyoxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1kcy1fn</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>What can I do to avoid bubbles in my mani?</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcy1fn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1kcxzxm</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Rogue Laquer Order Timeline?</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kcxzxm/rogue_laquer_order_timeline/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1kcxsdj</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Glitter grabber or just normal coat</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/17h1giqtkcye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1kcxd20</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>I got on Temu so it doesn’t have a name. Lol</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aj25iierfcye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1kcx5um</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>BCB Lacquers - Beyond The Reef Decals</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcx5um</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1kcwvrb</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>UK dupes for Mooncat's Jewel Beetle?</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kcwvrb/uk_dupes_for_mooncats_jewel_beetle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1kcwrv1</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Not sure if the color is for me...</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcwrv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1kcw683</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Did not expect my local supermarket to slay this hard</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kcw683</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1kdno39</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>need help choosing</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdno39</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1kdnhqk</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>I can't decide and I'm not satisfied</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdnhqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1kdmbbi</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Recent Sets from a DIY newbie</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdmbbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1kdk1bs</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Blues clues themed nails</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pkmkwiutphye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1kdjuhy</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>I usually do small easy designs on my mom and sister and today the both decided to challenge me with designs way above my skill level</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdjuhy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1kdi7fn</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Update: New and hopefully improved logo!</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdi7fn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1kdfqiq</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Are these nails too difficult for a local artist?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3il4czv4kgye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1kdfbho</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Nails 🖤</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/onx3d0riggye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1kdevkr</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>I made Littlest Pet Shop Nails!🌈✨</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdevkr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1kdelzs</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Red french</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/384flllfagye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1kdd55s</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Butterfly nails 💅🦋</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdd55s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1kd9luy</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>All my colors take a peak</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd9luy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1kd8v3h</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>strawberry nails 🍓</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd8v3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1kd8tye</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Flowah powah</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd8tye</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1kd5afh</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Cat's eye aura and relief effect, today's work</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd5afh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1kd55l2</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Love how they turned out &amp; love the colors, Happy spring 💜</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd55l2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1kd559v</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Any advice on how I can improve?</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u9uvg5h2aeye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1kck6c2</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Short ones☀️</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgkb0j3ln8ye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1kd29je</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Trying something new</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd29je</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1kd20sw</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>3d sculpted butterfly nail pair 🦋</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8bbv3k3pmdye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1kd164m</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>I love these even tho they are simple</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd164m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1kd0sdq</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>The Nails Bae Freestyle set. I’m back. What your thoughts?</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kd0sdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1kd03jk</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>I’m not okay, I promise.</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9idamck7dye1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun May  4 08:10:31 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_04.xlsx
+++ b/data/collected_data/2025_05_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1244"/>
+  <dimension ref="A1:C1433"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21581,6 +21581,3219 @@
         </is>
       </c>
     </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1kee4ly</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Cute ombre nails</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ej9t04tyvpye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1kedrnh</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>First time trying out press ons ☺️</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kedrnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1keczoe</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Is this the nude for me?</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1keczoe/is_this_the_nude_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1keciuf</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>How much are these press ons worth?</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swgu5o9bcpye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1kec0x7</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Rhinestone cherries 🍒 obsessed</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h91sn6le6pye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1kebief</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>What kind of manicure would you recommend? Want length but nails keep breaking.</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kebief/what_kind_of_manicure_would_you_recommend_want/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1kebsu4</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>another french set</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0r1njyt3pye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1kebkrr</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Animal print Nails.</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9tqiyia1pye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1keau6z</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>my graduation is in a week and i need some advice on my nail set!!!</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1keau6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1keaq4l</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Discoloration on big toe</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/de9yd694soye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1keb7jl</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Strawberry vibes 🍓</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1keb7jl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1keb59t</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>My fave set of nails ever!</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vl4ya3kiwoye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1kearuv</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Engagement Nails</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ordrhvimsoye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1keanon</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Pedicure while nail falling off?</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkvb530froye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1keaky4</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Almond or Square ?</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1keaky4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1kea4aj</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>love these pink cat eye press ons! 💕😍</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kea4aj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1kea3iy</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>fav press ons!! Best quality, I get 3+ weeks with none that have popped off!</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggnb2dciloye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1ke8fg9</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nsexdum4oye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1ke9nlj</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>I was told they look weird... Are they really rhat weirdly shaped?</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke9nlj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1ke9jfs</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>OPI comparison</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pe7t9vysfoye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1ke94nt</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>diy at home chrome recs?</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ke94nt/diy_at_home_chrome_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1ke756d</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Need help with cuticle prep?</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ke756d/need_help_with_cuticle_prep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1ke9doc</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Are these devices really useful?</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0saw5g4eoye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1ke7e3p</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Why does the skin under my nails look like this?</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5laxajnaunye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1ke9dd3</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Baby Croc and Ombré 🐊🐊</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egbqf141eoye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1ke9dcu</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>My nails</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke9dcu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1ke99md</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>I always went for plain colors but in Spain I made these and loved them.</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxovp7hzcoye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1ke8u87</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>My Artist Kills It Every Time</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3l9hbvfq8oye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1ke8qgq</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>my emotional support nail buddy! 🗣️💕</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke8qgq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1ke8pfi</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Jewel beetle nails</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke8pfi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1ke8ohd</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Be honest, would you chop or glue this situation? I’m stuck.</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke8ohd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1ke8nda</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>My first try with gel.</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cuckrgjs6oye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1ke8fpo</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>IT'S NEVER ENOUGH WHEN WE TALK ABOUT GLITTER ✨🌸🩷 I'm in love with my new flirty nails</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ghfm9yso4oye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1ke8dsx</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>NEW MONTH? NEW NAILS 🩷✨🌸🎀 SO MUCH SHINE, IN LOVE WITH THIS PINK COLOR</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tustnyh64oye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1ke8d8k</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>She killed the nails even though they aren't my normal stiletto shape 😍</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke8d8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1ke7vk0</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>How much do you pay?</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ke7vk0/how_much_do_you_pay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1ke7n3p</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Manicure</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wuv6i57rwnye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1ke7lwf</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Bees!</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qn7t48ofwnye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1ke72dz</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>In love with the French 🥰</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yff8eb96rnye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1ke6ysq</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>My Beatiful nails</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unbq3od8qnye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1ke6e4b</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Nails Sacrificed for the Garden</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3bktwm03lnye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1ke6blw</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>💗</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i35tweufknye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1ke500l</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>I’m kind of obsessed</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/utfirhps8nye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1ke5lr2</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Inspired, combined and reinterpreted</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1yb2qr3enye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1ke5r67</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>How to better describe to nail artist</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wi7y0giffnye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1ke5egd</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Chrome pedi nails</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/srb1ctpccnye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1ke544o</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>💙</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drlf1l9r9nye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1ke4w3k</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Update on my first Russian manicure</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mcvusgu7nye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1ke4sgs</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>How can I improve? What can I change?</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke4sgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1ke4ppg</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>I usually do medium or long nails on myself but these are so cute 💖</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yw50n90b6nye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1ke3sty</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Airbrush Gel cured on skin</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ke3sty/airbrush_gel_cured_on_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1ke4ft9</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>New Set.</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke4ft9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1ke4fkh</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Glamnetic Thumbnails</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ke4fkh/glamnetic_thumbnails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1ke4ena</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Zodiac Scorpio/water sign set</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqz370in3nye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1ke4csz</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Father-in-law first ever manicure! He asked for a friendly happy 🐳 😂</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w57ub9d73nye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1ke4amz</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Nausicaa cat eye!!</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kgzupzqp2nye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1ke49u4</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Natural nails enhanced</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke49u4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1ke46z8</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>What shape is a full acrylic set?</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ke46z8/what_shape_is_a_full_acrylic_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1ke451w</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>best manicure for long, natural nails?</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ke451w/best_manicure_for_long_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1ke43zr</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>How much do you tip your nail stylist?</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r56g2xw41nye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1ke42hj</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Salon Etiquette regarding a Plantar wart</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ke42hj/salon_etiquette_regarding_a_plantar_wart/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1kdzgkw</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>why is my nails kinda pale at the tip? it’s pale/white-ish at the end of the nail bed (before the grown nail)</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdzgkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1ke3que</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>My old nail sets from last year, when I started training to become a nail tech</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke3que</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1ke221k</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>How to find a gentle nail tech for gel nails</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ke221k/how_to_find_a_gentle_nail_tech_for_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1ke1q9g</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>how do you like these cat eye nails?</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke1q9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1ke1gdw</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>My nail girl popped off</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfwjb4nafmye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1ke01yt</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>I was inspired by an artist I see on YT and IG.</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke01yt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1kdzp7p</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Support?</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kdzp7p/support/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1ke3r0n</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>My pretty claws</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke3r0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1ke3ql0</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Old birthday nails ♓️</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vrevypk1ymye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1ke3pm5</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Let the nail tech pick the design.</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwcr11jtxmye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1ke3j5v</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Nail Refresh Saturday ✨🩷💅🏻</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ac93654bwmye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1ke3g6k</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Thunderbolts* Nails</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke3g6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1ke3fiw</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Men's nails are futile!</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qto9cihvmye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1ke3f3s</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Mismatched Set</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke3f3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1ke3b2v</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>new nails!✨️</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3pq0i9humye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1ke3ac2</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>New set Saturday 😍</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ke1hotfbumye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1ke33ws</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>💗💗💗</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke33ws</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1ke2wce</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Second try getting gel nails at home ❤️🌸</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7p2on1cpmye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1ke2fbb</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>First Manicure and I'm so upset</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke2fbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1ke1wfq</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Bugs n things</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke1wfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1ke1mei</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Simple nails for the kendrick lamar/SZA concert.</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4swyvhogmye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1ke1l6e</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>So i have been low key with my style and colors but i just need it</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jcv43f0egmye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1ke1c57</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Rate my beginner nails!</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke1c57</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1ke196x</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Junk nails 💅</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke196x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1ke18aj</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Just a little natural cat eye - no polish just sparkles ✨💫✨</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnb287zgdmye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1ke0pbv</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>I can't grow my nails no matter what I do</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ke0pbv/i_cant_grow_my_nails_no_matter_what_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1kdzio5</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>New nails 🍉 🍊 🍋 🍓</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qs6ngbq00mye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1kdzdt5</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>530 or 514?</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7uos2szylye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1kdz4nd</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Product question</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kdz4nd/product_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1kdyttf</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Nails are a fun little hobby. Did this set on myself</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1xnfh8rulye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1kdyfun</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Latte Art Manicure</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdyfun</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1kdydhf</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Builder gel on my mom. Her 2nd time. Nails are growing 🤭</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zemk58h8rlye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1kdyd51</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>A set im proud of💖</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdyd51</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1kduv76</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Fixing one nail vs getting whole set</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsooebohzkye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1kdqmp6</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0wdfjslwjye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1kdrgo9</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>What's wrong with my nails?</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zasjjali5kye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1kdoz2q</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>New Set, Today’s Color- Couture</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdoz2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1kdx45t</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>What's the longest you had to keep a set going ?</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdx45t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1kdxelj</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Is my nail going to fall off?</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dwu7xepjlye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1kecqix</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>5-6 months of growth</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kecqix</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1kebori</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Favorite Morgan Taylor polishes?</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kebori/favorite_morgan_taylor_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1keaqug</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>ILNP Polishes on brown skin + notso mini review</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1keaqug</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1keaakp</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Gel top coat under regular polish?</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1keaakp/gel_top_coat_under_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1kea8cr</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Crystal knockout “fly owl”</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kea8cr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1kea7dr</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>What I wore in April</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kea7dr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1kea3ls</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>oh god</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fxs5ksfloye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1ke9st9</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Cat`s eye effect</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rusa41l4ioye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1ke9qcw</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Clutch your pearls</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jnqsm7xqhoye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1ke9nm0</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Dupe for Sally Hansen Good Kind Pure in Lavender Haze???</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ke9nm0/dupe_for_sally_hansen_good_kind_pure_in_lavender/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1ke9iaf</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>OPI comparison</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jlenkavgfoye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1ke97lq</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>{PR} Meet Hot Damn Anthurium from Sassy Sauce Polish | PPU</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke97lq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1ke97ir</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Dupe for Mooncat's memento mori with cirque linen jelly and chrome powder</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sdukkifecoye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1ke7x5j</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Every week I tell myself this is my favorite</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke7x5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1ke7tme</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Hardeners, strengtheners, oils for brittle nails?</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ke7tme/hardeners_strengtheners_oils_for_brittle_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1ke7gd2</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Kiko Milano 497 / Chanel Taboo 593 dupes</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ke7gd2/kiko_milano_497_chanel_taboo_593_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1ke7bn3</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Spare Boxes</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnk10kemtnye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1ke7b7x</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Nailed the polish match for the tassel for my partner’s graduation</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rb9rc52itnye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1ke6yh6</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>The Perfect Gold Reflective Nail Polish 💅</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o1eujcf3qnye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1ke6q0g</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Happy Star Wars Day everyone (early)</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke6q0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1ke6j8j</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Why is my middle fingernail such an a-hole??</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke6j8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1ke6blp</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Bonnie B Magnetic Powder &amp; Regular Nail Polish</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ke6blp/bonnie_b_magnetic_powder_regular_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1ke2jaq</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Kimono Print🪷👘</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke2fn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1ke4o4n</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>I'm looking for a nail polish that matches this PS5 controller?</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ysjrz79o5nye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1ke63fx</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Looking for a specific type of glitter polish</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke63fx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1ke5zaw</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Mint is the color of spring 💖</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvedhuydhnye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1ke5u7m</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>If you missed Born Ugly from holo taco...</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke5u7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1ke5odd</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Do you care about the color difference when the whites of your natural nail show through?</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tgtxfj1renye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1ke5fq8</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>April manis 🐣</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke5fq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1ke4x6y</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>ooo lallaaa</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke4x6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1ke4th3</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Top and base coat recs?</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ke4th3/top_and_base_coat_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1ke4i7h</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Does anyone else have this same issue with Jen and Berries?</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ke4i7h/does_anyone_else_have_this_same_issue_with_jen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1ke4au8</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Goulish match 😊</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke4au8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1ke3qs5</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Non thermal UK match please?</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txsu3r03ymye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1ke3cq3</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Dazzle dry one week in… disappointed.</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dswi04kuumye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1ke31yg</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>one half "i just bought these and want to wear them all" skittle - one half bluegreen skittle (+ dog tax)</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke31yg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1ke2p94</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Comparing OPI and ILNP reds</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ke2p94/comparing_opi_and_ilnp_reds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1ke0vam</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Pull it Together under flash 📸</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gq8kso6iamye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1ke0v33</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>I found my type 💖</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/111cmuugamye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1ke0on0</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Polish wear update</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmtlizc29mye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1ke0lrt</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Butter yellow 🧈</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke0lrt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1ke0jwe</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Blue for days</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48hz04318mye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1ke0c39</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>April mani roundup 🌷🪻🌸</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke0c39</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1ke09hz</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Gettin in touch with my feminine side🤣</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqqgi7jt5mye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1ke05ca</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Fairycore 🧚</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke05ca</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1kdzqr5</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>blue water 💙🦋🐳🌀🩵💧</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdzqr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1kdzl3l</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Bees Knees Lacquer Dupe ?</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/njnlydlj0mye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1kdzkw7</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>I Scream Polish replacement brush?</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kdzkw7/i_scream_polish_replacement_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1kdz88l</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>💛❤️Thunderbolts*🖤*️⃣</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdz88l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1kdz69j</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Sabertooth 🐅 ❄️</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdz69j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1kdz3pz</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Psilocin 🍄</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4yxja7luwlye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1kdyn26</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>BKL combo</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/704ndm48tlye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1kdy0o5</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Walked by my neighbor's rose bush and caught a vibe</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdy0o5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1kdxtf5</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Gel X polka dots for spring :)</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ldpsauxmlye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1kdxnhr</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>obsessed with this combo 😍</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdxnhr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1kdxm6y</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Last longer?</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49bewgrellye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1kdxibw</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>New fav</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qmfmztiklye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1kdwxfq</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>wym you can’t believe I caved and ordered during the last 30 minutes of the lunar sale?</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdwxfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1kdwx1k</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Sparkley and moody</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdwx1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1kdwu7x</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Has anyone with a gel nail polish allergy gotten acrylics professionally without an allergic reaction?</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kdwu7x/has_anyone_with_a_gel_nail_polish_allergy_gotten/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1kdwgu2</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Look Into My Crystal Ball🔮</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdwgu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1kdwdzx</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>This polish may have ruined me for all others</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdwdzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1kdwcgd</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Growing out PVB damage, does anything help in the meantime?</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kdwcgd/growing_out_pvb_damage_does_anything_help_in_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1kdwcen</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Cracked - Lima Jelly Bean + reverse tips</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdwcen</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1kdv78l</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>vampy manicure in the spring bc no one can stop me 🧛🏿‍♀️</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m8bngyl52lye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1kdsx3t</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>My mooncat rainbow</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43rplmk8jkye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1kdsrop</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>iconic for a reason</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdsrop</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1kdrywm</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Antivenom held up through 8 hours of gardening!</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ymlbyxblakye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1kdrme3</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Dupe request</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdrme3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1kdqqcv</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Sour Apple Froggos</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vlk8tl5sxjye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1kdq8om</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Magnetic effect question</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4l6x0ob7sjye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1kdq4t1</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Sparkle and glooooww</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdq4t1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1kec3ci</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Got bored so did this</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kec3ci</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1kebowx</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Fresh new set!</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7hfl6ql2pye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1kea0cw</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Cute pink nails</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7job1iulkoye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1ke8nvz</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>By Request, Vintage Halloween set</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gt9rvley6oye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1ke6ifa</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Pierce the Veil nails</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpqfiug4mnye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1ke1vhe</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Rate my beginner nails!</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke1vhe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1ke1uxf</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Nail test for my wedding</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke1uxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1ke1tf6</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>I saw someone do these and I couldn’t stop thinking about it</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke1tf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1ke03c7</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>I was inspired by an artist I see on YT and IG.</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ke03c7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1kdzsif</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>inspo vs what I got 💞</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdzsif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1kdz5zu</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Obsessed with how these came out 🍋</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkdiur9cxlye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1kdxe51</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>today's work, blues ✨️</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdxe51</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1kdxbkb</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>que tal me quedo esta técnica</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wenitbrvilye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1kdvnd7</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Flamingos 🤩🤩</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdvnd7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1kdvn72</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>I’m still not that great at it yet no</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2bzw4pp5lye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1kdv73b</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Art nouveau set (little crooked in the picture but they don’t look crooked on my hands)</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kdv73b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1kde94x</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>NEED AN ARTIST IN MELBOURNE</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8luisyxg7gye1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>